<commit_message>
use general number format by default
</commit_message>
<xml_diff>
--- a/tests/testthat/_snaps/knitxl/data_frame.xlsx
+++ b/tests/testthat/_snaps/knitxl/data_frame.xlsx
@@ -388,11 +388,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>